<commit_message>
change to use sqlalchemy in import database
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="C60 db" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>ROW</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>JJ101</t>
+  </si>
+  <si>
+    <t>jq100 devices</t>
+  </si>
+  <si>
+    <t>Jq100</t>
+  </si>
+  <si>
+    <t>Jq150</t>
+  </si>
+  <si>
+    <t>Jq101</t>
   </si>
 </sst>
 </file>
@@ -98,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -131,7 +143,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +540,24 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" s="1"/>
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5467</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F7" s="1"/>
@@ -562,9 +591,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -583,6 +614,11 @@
         <v>21</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change the database is accessed with using sqlalchemy, except in the login section
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="C60 db" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>ROW</t>
   </si>
@@ -96,13 +96,16 @@
     <t>jq100 devices</t>
   </si>
   <si>
-    <t>Jq100</t>
-  </si>
-  <si>
-    <t>Jq150</t>
-  </si>
-  <si>
     <t>Jq101</t>
+  </si>
+  <si>
+    <t>jq100</t>
+  </si>
+  <si>
+    <t>jq150</t>
+  </si>
+  <si>
+    <t>100 devices</t>
   </si>
 </sst>
 </file>
@@ -141,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,10 +473,10 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -489,10 +493,10 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -509,10 +513,10 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -529,10 +533,10 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -549,18 +553,35 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" s="1"/>
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3456</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
+        <v>200</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" s="1"/>
@@ -593,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -616,7 +637,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>